<commit_message>
zzf 费控 后台 2021-04-20 16:24:37
</commit_message>
<xml_diff>
--- a/PD/v5/assets/public/商家导入模板.xlsx
+++ b/PD/v5/assets/public/商家导入模板.xlsx
@@ -1,60 +1,480 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
-  <workbookPr showInkAnnotation="0"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13433\Desktop\工作\物流费控\导入模板\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13433\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C89841B6-5BCB-4174-8B59-D23072098D32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B0EBB8-4E7E-4AE2-9578-F3E9D6C83F67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="商家信息数据" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t xml:space="preserve">商家名称    </t>
+    <t>*商家ID</t>
   </si>
   <si>
-    <t>余额预警值</t>
+    <t>*商家名称</t>
   </si>
   <si>
     <t>余额</t>
   </si>
   <si>
-    <t>商家ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>余额预警值</t>
+    <phoneticPr fontId="84" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <name val="宋体"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="86">
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -80,12 +500,261 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -105,7 +774,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -121,7 +790,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -133,7 +802,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -147,12 +816,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -180,14 +849,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -215,6 +901,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -357,72 +1060,164 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="18.19921875" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="1" max="4" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="25.05" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:4" ht="25.05" customHeight="1">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" ht="25.05" customHeight="1">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" spans="1:4" ht="25.05" customHeight="1">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+    </row>
+    <row r="5" spans="1:4" ht="25.05" customHeight="1">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19"/>
+    </row>
+    <row r="6" spans="1:4" ht="25.05" customHeight="1">
+      <c r="A6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="23"/>
+    </row>
+    <row r="7" spans="1:4" ht="25.05" customHeight="1">
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="27"/>
+    </row>
+    <row r="8" spans="1:4" ht="25.05" customHeight="1">
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="31"/>
+    </row>
+    <row r="9" spans="1:4" ht="25.05" customHeight="1">
+      <c r="A9" s="32"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="35"/>
+    </row>
+    <row r="10" spans="1:4" ht="25.05" customHeight="1">
+      <c r="A10" s="36"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="39"/>
+    </row>
+    <row r="11" spans="1:4" ht="25.05" customHeight="1">
+      <c r="A11" s="40"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="43"/>
+    </row>
+    <row r="12" spans="1:4" ht="25.05" customHeight="1">
+      <c r="A12" s="44"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="47"/>
+    </row>
+    <row r="13" spans="1:4" ht="25.05" customHeight="1">
+      <c r="A13" s="48"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="51"/>
+    </row>
+    <row r="14" spans="1:4" ht="25.05" customHeight="1">
+      <c r="A14" s="52"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="55"/>
+    </row>
+    <row r="15" spans="1:4" ht="25.05" customHeight="1">
+      <c r="A15" s="56"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="59"/>
+    </row>
+    <row r="16" spans="1:4" ht="25.05" customHeight="1">
+      <c r="A16" s="60"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="63"/>
+    </row>
+    <row r="17" spans="1:4" ht="25.05" customHeight="1">
+      <c r="A17" s="64"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="67"/>
+    </row>
+    <row r="18" spans="1:4" ht="25.05" customHeight="1">
+      <c r="A18" s="68"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="71"/>
+    </row>
+    <row r="19" spans="1:4" ht="25.05" customHeight="1">
+      <c r="A19" s="72"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="74"/>
+      <c r="D19" s="75"/>
+    </row>
+    <row r="20" spans="1:4" ht="25.05" customHeight="1">
+      <c r="A20" s="76"/>
+      <c r="B20" s="77"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="79"/>
+    </row>
+    <row r="21" spans="1:4" ht="25.05" customHeight="1">
+      <c r="A21" s="80"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="83"/>
+    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
+  <phoneticPr fontId="84" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>